<commit_message>
Sub to event for graph printing
</commit_message>
<xml_diff>
--- a/Extension/2017-2016-expenses.xlsx
+++ b/Extension/2017-2016-expenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\amazon-expense-extension\Extension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1FD85C-73C4-477E-89E4-7EF0C3DBE084}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526C356C-C9A7-45B4-945A-BE1C400E5603}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8FA5E6E8-3390-4C40-B4C8-CEF9373B2C5F}"/>
   </bookViews>
@@ -64,8 +64,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -380,176 +381,245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1927E0-187E-4F8A-938A-E733A521C9EB}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2017</v>
       </c>
       <c r="B1">
         <v>2016</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1">
+        <v>44292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10.45</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>7.88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13.9</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>41.65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>18.46</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>44.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14.61</v>
       </c>
       <c r="B5">
         <v>13.95</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4.28</v>
       </c>
       <c r="B6">
         <v>16.48</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>13.21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
       <c r="B7">
         <v>6.99</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>18.38</v>
       </c>
       <c r="B8">
         <v>5.07</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>54.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>19.95</v>
       </c>
       <c r="B9">
         <v>28.89</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12.84</v>
       </c>
       <c r="B10">
         <v>159.91</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>12.39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.1399999999999997</v>
       </c>
       <c r="B11">
         <v>4.93</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>14.99</v>
       </c>
       <c r="B12">
         <v>59.29</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>19.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>14.37</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>279.98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>23.98</v>
       </c>
       <c r="B14">
         <v>23.99</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>6.39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7.99</v>
       </c>
       <c r="B15">
         <v>144.74</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6.99</v>
       </c>
       <c r="B16">
         <v>93.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>14.54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>34.5</v>
       </c>
       <c r="B17">
         <v>5.98</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>37.04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>7.91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9.99</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>19.63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>72.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>SUM(A2:A22)</f>
         <v>310.22000000000003</v>
@@ -557,6 +627,65 @@
       <c r="B23">
         <f>SUM(B2:B22)</f>
         <v>564.12</v>
+      </c>
+      <c r="C23">
+        <v>15.99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>11.99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>27.69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>249.39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>39.840000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>41.93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>9.9700000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>66.709999999999994</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>16.989999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>14.97</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>13.99</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <f>SUM(C2:C33)</f>
+        <v>1110.46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>